<commit_message>
updated minutes of meeting
</commit_message>
<xml_diff>
--- a/Minutes_of_meeting/Minutes-of-meetings.xlsx
+++ b/Minutes_of_meeting/Minutes-of-meetings.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Desktop\UCD Practicals &amp; Projects\Summer Team Software Project\FInal Project Git\US-Stock-Options-Data-Pipeline-microservice\Minutes_of_meeting\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B3AE7FAB-23BD-4D49-8CED-19299605DEF4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E3A44CEE-0592-49F1-BDF5-04C7AC54FD83}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{B6626D02-EAB1-4E07-BCA0-63E94328CB3A}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>DATE</t>
   </si>
@@ -818,6 +818,79 @@
   <si>
     <t>1. Submitted all the required documents.
 2. Discussed further task for the upcoming team workshop.</t>
+  </si>
+  <si>
+    <t>1. Begin development of scheduling mechanisms and link them to respective services.
+2. Each team member to start implementing their assigned component (Collector, Processor, Writers).
+3. Set up and test Docker containers for each microservice.
+4. Use the drafted flow diagram as a blueprint for coding and system integration.
+5. Continue daily stand-ups or syncs to ensure blockers are addressed quickly.
+6. Start implementing the finalized data plan and track progress through Jira.
+7. Plan for next meeting to demo partial integration and review dashboard progress.</t>
+  </si>
+  <si>
+    <t>1. Team members encountered roadblocks while implementing parts of their tasks and required mutual support.
+2. Lack of clarity on the complete data pipeline structure initially caused minor confusion in scheduling and dependencies.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1. Identified and finalized the scheduling jobs required across services.
+2. Discussed the core methods/functions needed for:
+a. Collector: Data fetching strategy
+b. Processor: Data cleaning/transformation logic
+c. Writers: Database and file output handling
+3. Discussed and initiated setup for the Dockerfile for containerization.
+4. Designed a rough flow diagram outlining interactions between five key services:
+a. Scheduler
+b. Collector
+c. Processor
+d. DB Writer
+e. File Writer
+5. Assigned specific responsibilities to each team member and updated the Jira board accordingly.
+6. Discussed how options data should be presented on the dashboard for clear visibility.
+7. Finalized the data flow plan for implementation.
+</t>
+  </si>
+  <si>
+    <t>1. Finalize the data model including:
+a. Columns for each table
+b. Indexing strategy for PostgreSQL
+c. Schema for time-series storage in InfluxDB
+2. Team members to prototype database setup on:
+a. Azure PostgreSQL instance
+b. InfluxDB local/cloud setup
+c. S3 bucket configuration for historical data
+3. Begin integrating Kafka into the architecture for event-driven communication between services.
+4. Start setting up Prometheus and Grafana monitoring stack.
+5. Define how Dockerfiles will be structured per microservice and set up Kubernetes manifests.
+6. UI team to start wireframing frontend components using React based on yFinance reference.
+7. Finalize decision on storing historical data — static tables vs. S3 — based on access needs and performance.
+8. Implement the initial version of the writer service to create and update the necessary databases.</t>
+  </si>
+  <si>
+    <t>1. Evaluated various database options based on use cases:
+a. PostgreSQL for relational/day-wise data
+b. InfluxDB for time-series data
+c. S3 for storing large CSV files and historical data
+2. Team members explored different service providers:
+a. Azure (Postgres hosting)
+b. AWS (S3, RDS)
+c. Google Cloud
+d. InfluxDB Cloud
+3. Kafka’s role in microservice communication was discussed, along with strategies for integration.
+4. Defined key fields and discussed schema/data model design for the database.
+5. Importance of indexing in PostgreSQL to improve query performance was emphasized.
+6. UI/UX planning began with reference to yFinance, to be implemented using React.
+7. Discussion on using Prometheus and Grafana for monitoring and data visualization.
+8. Talked through Dockerfile structure for microservices and deployment using Kubernetes.
+9. Clarified roles of PostgreSQL vs. InfluxDB for frontend visualizations and real-time data insights.
+10. Debated between using S3 or a static PostgreSQL table for storing historical data.
+11. Agreed that databases will be initialized and managed via the writer service.</t>
+  </si>
+  <si>
+    <t>1. Uncertainty about which database services best fit different types of data (e.g., historical vs. day-wise).
+2. Performance concerns with PostgreSQL for large datasets — indexing strategies need optimization.
+3. Need for clarity on Kafka integration across microservices.
+4. Complexity in deciding where and how to store long-term historical data — S3 vs. static PostgreSQL tables.</t>
   </si>
 </sst>
 </file>
@@ -873,7 +946,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="2" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
@@ -895,6 +968,9 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1210,10 +1286,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0C4CB3A1-9D53-459A-9590-285823EBD908}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+    <sheetView tabSelected="1" topLeftCell="A8" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,6 +1379,52 @@
         <v>18</v>
       </c>
     </row>
+    <row r="7" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="5">
+        <v>45820</v>
+      </c>
+      <c r="B7" s="8" t="s">
+        <v>24</v>
+      </c>
+      <c r="C7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="409.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="5">
+        <v>45821</v>
+      </c>
+      <c r="B8" s="8" t="s">
+        <v>20</v>
+      </c>
+      <c r="C8" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" s="5">
+        <v>45824</v>
+      </c>
+      <c r="B9"/>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B10"/>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B11"/>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B12"/>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="B13"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>